<commit_message>
Get daily reddit data: Tue Mar 26 08:07:52 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_03_31.xlsx
+++ b/data/2024_03_31.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C443"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,2420 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1bo1zh6</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Holo is life ⭐️</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bo1zh6</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1bo1ecd</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>i’m sure you know the question 🤣</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bo1ecd</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1bo0pzq</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>🩷🤍🩷</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ck8yyd8tdmqc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1bo0asl</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel extensions </t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bo0asl/gel_extensions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1bnz3k6</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Easter nails </t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qmzfpv47wlqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1bnypa6</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Peeling</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j4ndyj2bslqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1bny44f</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>how’d i do?</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3g3xas1vmlqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1bnxyci</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Cute 😍</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g3831wedllqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1bnxxbw</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Cutsie and dog themed</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnxxbw</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1bnw09k</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Pink chrome fill today 🩷</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nyotcaoq4lqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1bnvaw7</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nothing crazy, but my first at home gel manicure </t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d8lspiaxykqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1bnukpo</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Day 1 of 30 day nail detox</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnukpo</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1bnu37k</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>How long for this to grow back?</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1w4d14apkqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1bnsgfs</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Went to get a Russian manicure and was turned away</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bnsgfs/went_to_get_a_russian_manicure_and_was_turned_away/</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1bnsctm</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thumb nail splitting </t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bnsctm/thumb_nail_splitting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1bnufek</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Does pushing the cuticle elongate the nail bed??</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bnufek/does_pushing_the_cuticle_elongate_the_nail_bed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1bnubvx</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>New fill in!</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6jc4qhg6rkqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1bnttip</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>My birthday nails as a spring baby</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tzcqgtp6nkqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1bntf9q</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>recently stopped biting my nails after being a lifelong nailbiter... i know its nothing much, but i am proud of myself..</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ob4yhu5akkqc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1bntcq7</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Did my sisters nails &lt;3 easter colors of her choosing</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bntcq7</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1bnsvl9</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>What nail shape fits my hands?</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnsvl9</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1bns5ti</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>age old debate…</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bns5ti</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1bns1a4</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Speckled egg nails for Easter 🐣 </t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kowty6dy9kqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1bnrue0</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Bridal nails 🥳🥳</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnrue0</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1bnrqon</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>finally got my fill after 4 weeks 🤧</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnrqon</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1bnrg9h</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>First time trying gel nail polish (on my natural nails)</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnrg9h</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1bnqort</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>DIY "refills" when you live in a remote community and cannot always go to salon every 3 weeks (swipe for before)</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnqort</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1bnqi38</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Which shape suits my fingers better?</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnqi38</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1bnpr86</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Any tips on how to make the border of the 3D art more clear?</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnpr86</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1bnpjup</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Celestial spring</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnpjup</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1bnp4w8</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is it too early for corals/neons? </t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/84dzos1vpjqc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1bnonm9</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Of course my palate cleanser is holographic</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l9kscxjkmjqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1bnm2hw</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>My work 🥹 how do you rate them?</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnm2hw</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1bnkwyu</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>First Timer</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bnkwyu/first_timer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1bnks0e</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Can I use UV gel glue for gems on my natural nails?</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bnks0e/can_i_use_uv_gel_glue_for_gems_on_my_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1bnnwkt</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>A dad on a mission. My daughter continues her trend with curves.</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnnwkt</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1bnnp2f</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails i did! </t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qwkub4zzfjqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1bnnl35</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>My DIY nail art design 🧡</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnnl35</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1bnmz6f</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Buying gel polish as a non-professional?</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bnmz6f/buying_gel_polish_as_a_nonprofessional/</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1bnmyb7</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Had to get the perfect photo 🇫🇷</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tsc4z0qwajqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1bnm3qn</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Fresh set ☘️</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnm3qn</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1bnlzch</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Easter eggs 🐣🐰 </t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/it1tg7i74jqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1bnlv8c</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Very delicate this time, but I think they are too long.</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/44rf09de3jqc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1bnkn1a</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Using nail glue as base</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bnkn1a/using_nail_glue_as_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1bnkj7r</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>My favorite chromes/pearls so far</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnkj7r</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1bnjy9y</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Blue Blue Blue 💙</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z7f4b8nvpiqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1bnifxb</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Questions after educating myself</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bnifxb/questions_after_educating_myself/</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1bnisf6</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>My Little Mermaid inspired nails</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnisf6</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1bnji07</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Easter!!</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnji07</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1bnj4e5</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>fave set</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnj4e5</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1bnj2s8</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>slayy</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b1jtqdtrjiqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1bniuao</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Lives up to its name!</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bniuao</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1bnil6y</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Sent the cursed pose to my family chat</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v9u5pk3agiqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1bnigpo</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Does pearl chrome powder show up on different color bases?!</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bnigpo/does_pearl_chrome_powder_show_up_on_different/</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1bni6eq</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>quick sparkly french on my natural nails🫧☁️🤍</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7j24z58adiqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1bnhwya</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Roller Rink</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tu8omqmfbiqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1bnhovw</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>pre flight mani 🛫</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4eca7y4r9iqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1bnh0yu</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>It’s only been 9 days, why do they look like this?</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnh0yu</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1bne38i</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>My spring nails, inspired by another redditor</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lzuj1bbwihqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1bnb5q8</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Less than 2 weeks and they have to come off for a job interview🥲 inspo from u/justagirl0723 !</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnb5q8</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1bn8wj0</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>biab journey 2024! jan - march</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bn8wj0</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1bng2en</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Gummy bear charms! 🧸🫧🤍</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h4ij7qeuxhqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1bnfuik</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>I have just finished 5 mistakes! :D</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jm8u4ff7whqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1bnfq4l</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>They’re a little stained from henna :)</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5iw9io4dvhqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1bnfa0g</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jason nails! </t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jkgsdyjwrhqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1bnf0xd</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>I like to add accessories to my nails, does this happen to anyone else?</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nai27ptzphqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1bnex30</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>A simple birthday look🦋</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gwqsy896phqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1bnevt1</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Short nails</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tmcsx3wwohqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1bnco1h</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Unhappy with my nails but worried about going back and asking to have them fixed.</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnco1h</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1bnbsds</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Acrylic paint with a clear coat of nail polish??</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bnbsds/acrylic_paint_with_a_clear_coat_of_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1bnb55l</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simple spring nails for todays client. </t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kottkggcsgqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1bnabsz</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>hard gel cracked after 2 days?</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bnabsz/hard_gel_cracked_after_2_days/</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1bn9hx6</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>3 months of nail growth</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bn9hx6</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1bn8ls5</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Gel lack on natural nails, did them myself</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bn8ls5</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1bo20vw</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Holo is life ⭐️</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bo20vw</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1bnzqlj</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>How many coats of holo polish?</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bnzqlj/how_many_coats_of_holo_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1bnw1se</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Color help?</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bnw1se/color_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1bnzctp</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>First try at modern</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnzctp</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1bnz9gc</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>What's Your Favorite Scary Movie?</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnz9gc</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1bnyh9m</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>*sobs* nail break</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wkaj2vp8qlqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1bnwaqa</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Renouncing Spring and all his works featuring vintage bar glitter</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnwaqa</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1bnvkxi</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Enjoying this black holo polish before I clip all my nails down later. I broke four of them and more are on the brink of death😔 At least I’m already wearing black for their funeral. Cityscape by ILNP.</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnvkxi</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1bnv39s</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>LA Colors - Dream Chaser</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnv39s</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1bnugdu</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>My go-to nails</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0occndr5skqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1bntxce</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Not very spring like but I wanted something dramatic </t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x38w8esznkqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1bntvlq</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Last Winter Mani…..</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lq9avj7mnkqc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1bntr0v</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Husband picked these colors :)</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bntr0v</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1bntb2y</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Cirque Lucky Jelly</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bntb2y</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1bnt0d7</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>A must for pink lovers</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnt0d7</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1bnsdfm</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Rave: 10 day old manicure</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bn8tn7agckqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1bns9sc</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Looks better in IRL...like me</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bns9sc</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1bnrqff</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Dazzle Dry Help</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bnrqff/dazzle_dry_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1bnqm6z</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Rorschach pattern didn't turn out quite right, but I'm still happy </t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jgkhfw6xzjqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1bnqan3</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>💜🩶</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnqan3</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1bnq29n</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Best top coat to hold velvet effect?</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bnq29n/best_top_coat_to_hold_velvet_effect/</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1bnpqwt</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>First time trying nail art</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnpqwt</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1bnp8c1</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Playing with magnets ( aka whyyyy are shimmers so hard to photograph)</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnp8c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1bnoufq</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>I don’t usually go for lighter colors</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnoufq</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1bnoswh</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>🦋🔱🧞‍♂️⭐️🫐</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnoswh</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1bnoau9</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Major Batman and Robin vibes! (Old school! Lol)</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y48et3v6kjqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1bnoaje</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>What polish exudes this vibe?</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/paixpvw4kjqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1bno3if</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>ILNP Arctic Lights</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bno3if</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1bnni62</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Tried to convince myself I don’t need any of the new Cuticula polishes by swatching one I already own…it did nOT WORK</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vno0iainejqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1bnnbcc</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Ethereal Lacquer "Howl's Moving Castle" Collection Shipping?</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bnnbcc/ethereal_lacquer_howls_moving_castle_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1bnmvt2</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Testing out blues for my “something blue”</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pav4yqlfajqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1bnmepb</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>🐛Very Hungry Caterpillar 🐛</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnmepb</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1bnmbyr</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>There was an attempt at Ombré Easter Eggs</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rcu3k96n6jqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1bnm4gy</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>We don't talk about the right hand</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/187wz3q75jqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1bnlcuy</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Farm fresh eggs 🥚 🐓</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n24jclytziqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1bnkx3h</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>You're Finally Awake</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnkx3h</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1bnkv3b</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Painted My Nephew's Nails Today!</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnkv3b</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1bnjosf</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Two free magnet= Magic 🪄</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/89ap6vy0oiqc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1bnitcw</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Blue Jelly Sandwich Skittle 🪼🍞</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tow3wmtwhiqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1bnhr93</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Petals for a narcissist </t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/89qcngu8aiqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1bnhpoj</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Day 5, no touchups 😳 😍</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnhpoj</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1bnho64</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>I'm not good at this but this color is gorgeous</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bnho64/im_not_good_at_this_but_this_color_is_gorgeous/</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1bnhnan</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>pre flight mani 🛫</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0sqbki8f9iqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1bnhihs</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Violet is the vibe 💅🏻💜</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kl4kvlhf8iqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1bnhgjv</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>So I cannot find this polish online anywhere!!?</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnhgjv</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1bnh5ax</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>This heart had me SWEATING</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnh5ax</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1bnb64v</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone with experience of using LA Colors Nail polishes? </t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bnb64v/anyone_with_experience_of_using_la_colors_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1bnesie</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Little King Trash Mouth 🦝</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnesie</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1bnesco</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Marsala Jelly</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnesco</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1bneod3</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Swatch Request: Please help me avoid buying polish I have dupes for</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bneod3/swatch_request_please_help_me_avoid_buying_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1bncn3f</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Loud Lacquer?</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bncn3f/loud_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1bnammj</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Desperate times call for desperate measures</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qxt4oe1zmgqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1bn9wbu</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bn9wbu/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1bn8fnu</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Is this blurple? What is blurple?</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n6hm697zvfqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1bo0uwt</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>kawaii junk nails!</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bo0uwt</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1bo0cbi</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Not for sale💫🌞</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/69tt3nme9mqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1bnzduk</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Modern attempt - verdict pretty good</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnzduk</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1bnxga8</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Zebra Nails 🦓 </t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a2s177kyglqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1bnwalm</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Love my new manicure. Took me four hours.</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mbgt7r9z6lqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1bnw0de</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Cherry Blossom Nails</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnw0de</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1bnvwb6</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Did some funky clown nails</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oaq0nnwu3lqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1bnobc5</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>An order I made recently. Obsessed with the top set</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kecjqt9akjqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1bnm1dw</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>I'm in love with them ☺️</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnm1dw</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1bnlf8w</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Guess how I got this effect?</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pi1w50hb0jqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1bnkoll</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Think I really need to book a trip! </t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jjxu2p62viqc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1bnj4tp</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>2 hour set !! - First time doing nails other than my own! Let me know what you think &lt;3</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bnj4tp</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1bni5zr</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>What do you guys call this kind of design?</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bni5zr</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1bn8jeq</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Traditional look</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k0xe0eicxfqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Mar 27 08:07:53 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_03_31.xlsx
+++ b/data/2024_03_31.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C443"/>
+  <dimension ref="A1:C603"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7964,6 +7964,2726 @@
         </is>
       </c>
     </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1bov9d9</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>had a car event to go to so flames seemed fitting</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bov9d9</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1bov83z</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Need help with starting</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bov83z/need_help_with_starting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1boujz9</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Easter nails 🐣</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1boujz9</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1bouisi</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>What shape suits me better? ♥️</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bouisi</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1botm5e</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Nails for the week</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1botm5e</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1bosqsx</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>i honestly wish i could just keep them like this sometimes, idk why but i like the vibe. anyway suggestions please? i want to them to look scary. not color scheme scary, but like unsettling scary. idk how to explain it but i also don’t know how to execute it. sorry for being vague lmao.</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y38c8z31wsqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1bosack</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Nailssss</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bosack</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1bop9z6</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Best way to add another coat on already done gel nails?</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jn4jtbbi2sqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1booei3</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Best manicure I've ever gotten!</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1booei3</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1bokif4</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Nails for Spring</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bokif4</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1bokbd2</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Starting gel nails with cheap products</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bokbd2/starting_gel_nails_with_cheap_products/</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1boka7p</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>I am confused on strengthening basecoats, can I use this one as a perma base coat?</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1boka7p/i_am_confused_on_strengthening_basecoats_can_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1bojp62</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>anyone know what builder gel this is?</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bfqvtwv3yqqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1boh4g0</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Why do my nails do this?</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p8yeiv70gqqc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1bogiju</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Please help me choose 1 or 2, or neither</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bogiju</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1bor71y</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Gel strips on a lazy day~</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dt0fl2daisqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1bor5d5</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>press ons I made!</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bor5d5</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1boqwbz</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Fresh Set 💕</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1boqwbz</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1boqsdh</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Easter nails!</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q18r6mkuesqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1boq7c4</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bday nails are ready for next week </t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wev3kqk2asqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1boq2c0</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>How long does gel polish last as compared to dip?</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1boq2c0/how_long_does_gel_polish_last_as_compared_to_dip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1booble</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Lifting, help!!</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1booble/lifting_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1bonwss</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>francesita 💙🩷</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l4ofh4xxrrqc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1bonq9i</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>new set</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bonq9i</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1bonpk5</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>I’ve declared 2024 to be the year of chrome</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qc8ah7agqrqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1bon03a</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>In my Barbie era.</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jxpk4z1clrqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1bomlz8</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Red and Milky Way♥️🥛✨</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bomlz8</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1bom11d</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Chanel Taboo</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bom11d</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1bolzqb</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>A little palette cleanser.</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cqc9zkg6erqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1bolnff</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Springtime beauties</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bolnff</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1bolke5</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Dam Nail Polish - Cookie Recipe Swap 🍪</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bolke5</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1bokr25</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Gel nail colors that match these?</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bokr25</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1bokgy5</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>new set🥰</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r33kjldi3rqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1bojxdk</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>A Springy Mani for Everything</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5yoo4d5pzqqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1bojx9k</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>First Time Chrome DIY</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bojx9k</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1boimux</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do you think? Self-proclaimed nail tech LOL </t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vcajmxaqqqqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1boih7o</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>March nails</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1boih7o</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1bohud2</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>keroppi sanrio nails! 💚</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bohud2</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1bohqg2</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>🍋🍋🍋☺️</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tdb6no2ekqqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1bohp9k</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Spring nails</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bohp9k</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1bohezo</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Really been into simple sets lately. Have been doing my own nails about a year now. Builder gel on natural nail</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bohezo</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1boh4zb</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>How do they look on me? In smoke effect acrylic</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1boh4zb</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1bogzzw</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Spring nails!</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/izqyh616fqqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1bogrop</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>nail art advice</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/izx1fvzidqqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1bogohq</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Daisies! </t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zvyk2w3ucqqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1bogh02</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>I love the thumbs on this set especially!</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bogh02</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1bog7un</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>They remind me of fairy wings✨</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bog7un</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1bog31w</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What are some current nail art/nail trends that you hate? </t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bog31w/what_are_some_current_nail_artnail_trends_that/</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1bofwpd</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Best Inexpensive Press Ons for Wide Nails? (included pic of dress if anyone also has color reccs)</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j4cl11vl7qqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1bofmo6</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Help with gel nails at home</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bofmo6/help_with_gel_nails_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1bofk8q</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>6 weeks ago I stopped biting my nails. Today a stranger complimented my nails in public. What a ride</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6l3vkgg25qqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1bofc55</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Retro spring patterns</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bofc55</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1bocy54</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>How do I heal the skin around my nails?</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/glx7izlimpqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1boep30</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Not great application, but oh so holo.  </t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i1rupldyypqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1boein9</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Drastic color change indoors vs outide</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1boein9/drastic_color_change_indoors_vs_outide/</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1boe87d</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Orange Squiggles!</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/epsrq84ovpqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1bodou3</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>gel polish never sticks no matter what i do! help?</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h4rfkrxsrpqc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1bodl9w</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Removing gel acrylics </t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bodl9w/removing_gel_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1bodirs</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>is this normal?</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7dbfyjfmqpqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1bodeli</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Changed my nails after suggestions on my last post here</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bodeli</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1bod9vi</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Looking For Specific Nail Polish Instagram Influencer</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bod9vi/looking_for_specific_nail_polish_instagram/</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1bocvth</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Made these myself 💚💜 full cover tips with acrylic overlay. L.A. color (green) 'hint of Grinch' (purple) 'candy cloud'</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bocvth</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1bocpsd</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>still practicing. first time applying french tip outline.</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hs6zzizukpqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1bocnsg</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>What can I do if I want to change color without a complete fill?</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bocnsg/what_can_i_do_if_i_want_to_change_color_without_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1bocf9l</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Grafitti serie -part 1</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bocf9l</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1bocb39</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Anyone notice their nails grow faster on one hand than the other?</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bocb39/anyone_notice_their_nails_grow_faster_on_one_hand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1bobzv7</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>My second attempt with polygel</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bobzv7</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1bobx2q</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>French tips with a twist</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kfwltnx1fpqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1bo91me</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I did these nails, the color red is my favorite... anyone else fans of the color red? ha ha </t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7az93u6dtoqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1boatk9</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>What do you think of my spring nails? :)</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7769x5qx6pqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1boa2yp</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Last appointment with my nail tech before i move out of state 😭</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/awbxtucc1pqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1boa2vl</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Help fixing a cracked (natural) nail!</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4y6u2nfb1pqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1bo96d4</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Practice pop off set 🩷</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bo96d4</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1bo8y7l</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Newest set</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bo8y7l</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1bo8ua5</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>little pastel easter egg nails</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aoaanjnrroqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1bo8fj3</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Just found this sub! So happy 💃</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dkpd8mlnooqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1bo8dib</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>got my nails done ♡</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5v922qe7ooqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1bo87p2</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Love</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/osokq7ewmoqc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1bo837z</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>I hate them so much, I have never seen them do the magnetic like this! I wanna rip them all off</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f6cjiyqvloqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1bo77y7</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Love you all!!</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t0y545ykeoqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1bo6sih</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Reformed nail biter!</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bo6sih</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1bo6aay</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Tried doing my own nails. No equipment used</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yguxh7w36oqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1bo4689</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Simple Red DIY gel nails❤️</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04iaqvfyjnqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1bo33t2</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>First time ever with making nails. How did I do?</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bo33t2</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1bow9b4</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Let's Raise the Dead</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/35szn48kztqc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1bovqbm</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Emily de molly top coats </t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bovqbm/emily_de_molly_top_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1bov7pm</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Question for picking a nail color</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bov7pm/question_for_picking_a_nail_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1bou66y</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Looking for a milky white lacquer (gel appearance) similar to funny bunny by opi</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bou66y/looking_for_a_milky_white_lacquer_gel_appearance/</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1botvlx</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>For anyone who likes to track their collection with spreadsheets, how do you classify by colour? I think I messed mine up by categorising multicoloured polishes under all colours instead of just the dominant one</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wz7ursoh7tqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1bota3y</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Dream within a Dream ✨</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bota3y</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1bot6nx</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer - A Formidable Opponent</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bot6nx</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1bosvd9</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>How can I shorten Gel X nails? Got them done recently but I can’t stand the length. Can they be filed with a regular file without getting ruined?</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bosvd9</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1borx7h</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Which shape?</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1borx7h</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1boripe</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Request-- Verdigris?</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1boripe/request_verdigris/</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1boq3b1</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Velvet Nails / Biblically Accurate Magnet</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1boq3b1</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1bop1kq</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Orly In a Snap yellowing</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bop1kq/orly_in_a_snap_yellowing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1boou3k</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t xml:space="preserve">*cries* Another broken nail </t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1boou3k/cries_another_broken_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1boo3h8</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Was gifted the ella+milla cuticle oil pen. What do you guys think of it?</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1boo3h8/was_gifted_the_ellamilla_cuticle_oil_pen_what_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1bonet9</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>holo peri-social is here</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bonet9</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1bonc7o</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Shimmer shimmer</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mq84ppurnrqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1bon33f</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Week 3 of doing my own nails</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ugme6zaxlrqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1bomwc6</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>I swear your car always has the best lighting 😩</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bomwc6</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1bomvlo</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>I think I found a dupe…</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bomvlo</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1bolvmn</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Palette cleanser for your viewing pleasure😌🌤️</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/c648u49adrqc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1bolpgd</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>I've shown this one before but screw it!</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qthjcrw4crqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1bolm0r</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Dam Nail Polish - Cookie Recipe Swap 🍪</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bolm0r</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1boljm4</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Underrated ILNP color</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/epdhxv61brqc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1bol59f</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>💙 YES, this what Dreams Are Made Of!</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bol59f</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1bok3k4</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>What to do with this broken corner</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bok3k4</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1bojupu</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Springy Mani for a Lot of Events</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jsulgh56zqqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1bojucf</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>What is this style called if I wanted to ask a nail place if they were able to do it?</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gm2tla0ryqqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1bojgsb</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Trying my 1st LynBDesigns polish after this sub tipped me off a few weeks back. Matter of A Pinion</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0nrikvzhwqqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1bojfm8</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Am I being too impatient?</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bojfm8/am_i_being_too_impatient/</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1boigyc</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>My first LynB order!</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1boigyc</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1boiay9</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>I feel like it’s missing something… Am I wrong?</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6zpnk5fdoqqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1bohg5p</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>I clearly have a type... (swatches/comparison)</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/4YrRc5P</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1bogvgc</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Nail art advice</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yru6llc9eqqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1bogo6m</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Attempted Raindrops</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bogo6m</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1bof5g3</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Did I miss the Mooncat sale?</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bof5g3/did_i_miss_the_mooncat_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1boevao</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Beginner - Essie Island Hopping</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1boevao</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1boejwp</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Phoenix Elijah</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1boejwp</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1boecgx</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Slept on Essie sheers but now I am AWAKE</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gmdzrrgiwpqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1boe0bh</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Cirque price increase?</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sq5zcm35upqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1bodzba</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dupes for ILNP multichrome flakes </t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bodzba/dupes_for_ilnp_multichrome_flakes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1bodxu1</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>My little take on a spring mani! Wraps x polish</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lwwdvijmtpqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1bodhoi</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Diane von Furstenberg for Target x Sally Hansen Miracle Gel Nail Polish in Green Lust</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1jt5704fqpqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1bod8qi</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Pink/purple skittle!</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bod8qi</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1bod0h5</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>March ‘24 Blue Skittle 🫐</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bod0h5</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1boco4z</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>i hate this nail so much 😀😂🥲</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1yxw2kuikpqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1boclqe</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Don’t ask me how long these took</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1boclqe</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1bocjtb</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Normalize showing up to work with only three half-finished long nails because you decided to break out the paper forms at 10pm 😤</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bocjtb</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1boc9ij</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t xml:space="preserve">As a life long nail biter, I’m proud of my nail growth! </t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1b09cgakhpqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1boc4xv</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sob 😭 😭 </t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dgexb0zngpqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1bobsmy</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Favorite early Spring polish</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bobsmy</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1bobrfb</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Thank you to whoever suggested Orly's Nail Rescue kit</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bobrfb</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1bobmii</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Filing the top of polished nails? I know I'm the crazy one but just how crazy + request recommendations</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bobmii/filing_the_top_of_polished_nails_i_know_im_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1bob1oj</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>speckled egg frenchie</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4oq4zo7m8pqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1boac2n</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My partner lets me test out new varnish on him 🙄😂 </t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u81jug093pqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1boa19u</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>🔥💀Helldivers 2💀🔥</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1boa19u</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1bo9ylb</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Fairy Dust plus a couple of complimentary shades…💕🧚‍♀️</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bo9ylb</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1bo9ekb</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>“Besties” from Lumen (March ‘24 PPU)</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bo9ekb</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1bo8khp</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>little pastel easter egg nails</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w0ayc3ufpoqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1bo7me0</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>🎶 Hey Now, Hey Now! 🎶</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bo7me0</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1bo7dnq</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Help me find this color!</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bo7dnq</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1bovmpi</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>I'm obsessed with stars</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bovmpi</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1bovipl</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Attempted to do my own nails</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bovipl</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1bos72u</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Did these marble nails</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6dh95aazqsqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1boptgw</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>I made these</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1boptgw</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1booh8w</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>I'm in love with this design!</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1booh8w</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1bol7hd</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Red Spring Press on Nails</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bol7hd</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1bojw0s</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>I’m a beginner so these aren’t that good but I’m getting better.</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/skzsw0yezqqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1bojqa6</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>did this yesterday :D</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x8ldu3lbyqqc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1boj9ti</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>I did some cute speckled easter eggs as inspiration. Its really hard to do imperfect perfect dots. Also, how does one get the black to stop bleeding through or will I just have to suck it up?</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1boj9ti</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1boixwg</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Excited to finally find a group of my kind of peeps!</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1boixwg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1boir5c</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Did something simple for spring</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1boir5c</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1bohs9f</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>spring + leap year = keroppi nails! 💚</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bohs9f</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1bofqlk</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>This is my best set yet</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bofqlk</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1boelw0</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Little self love </t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gmded1fcypqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1bochbg</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Graffiti serie - part 1</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bochbg</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1bo8a5q</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Simple Easter nails. I think they came out cute 🥺</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k9efdihgnoqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Mar 28 08:07:52 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_03_31.xlsx
+++ b/data/2024_03_31.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C603"/>
+  <dimension ref="A1:C742"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10684,6 +10684,2369 @@
         </is>
       </c>
     </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1bppt93</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>wanted a fun excuse to use blue, so i painted on some fish 🐟</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j4pb6uac41rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1bpp7pa</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>They were supposed to be smiley faces but couldn’t get the mouth right so here we are ¯\_(ツ)_/¯</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpp7pa</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1bpoyyt</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Classic press on frenchies 💅</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o44dj05zt0rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1bpnoje</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>nails before cutting them</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/deq5apoye0rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1bpn3ft</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Ladybugs</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1s0t6xkq80rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1bpmtab</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>I’m soooo happy! ♥️</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpmtab</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1bpml2s</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Feeling a little 90's vibe with these 🩷❕️</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gytv5bxm30rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1bpmgl9</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Miss Saigon-ish nails</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpmgl9</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1bpm2rc</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>What shape do my nails look best in?</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpm2rc</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1bplow0</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Brown staining on dip? </t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5txorge5vzqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1bpjuty</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Went to the salon again. Mermaid scales! 🧜‍♀️</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpjuty</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1bpjh7p</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>💜✨</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jogjjftybzqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1bpjdrx</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Pearl accents</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u85w2dw5bzqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1bpj9kz</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Question on builder gel</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bpj9kz/question_on_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1bpiuax</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>I’m a sucker for a pink and black mani 🩷🖤</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpiuax</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1bpiiko</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>I think this is my favorite set yet.</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k97pre8w3zqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1bphuov</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Butterfly nails on myself</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e0tckqpiyyqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1bph9j9</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Barbie pink holo for spring!💖🌈</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bph9j9</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1bph51l</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>New set ✨</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bph51l</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1bpgwbv</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t xml:space="preserve">💅How did you increase speed during school? </t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bpgwbv/how_did_you_increase_speed_during_school/</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1bpgbjm</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Spring colors</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vyxjcqvvmyqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1bpfp2x</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>I need help iam a newbe</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpfp2x</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1bpexdm</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Gel over dip?</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bpexdm/gel_over_dip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1bpe1rm</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Sharing my soft spring nails</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpe1rm</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1bpdh8v</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Red😍</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y1zpeu372yqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1bpd68q</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>I haven't gotten my nails done in a year I feel so pampered</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4kg0ys000yqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1bpcxyp</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Springy nails!!</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/weppdyg9yxqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1bpctko</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Need tips to grow my nails</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bpctko/need_tips_to_grow_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1bpciyx</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Nail length</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ncf5jwbvxqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1bpbazz</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>a 15yo did these! $45</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpbazz</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1bpaz90</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Dragon Scales 🐉</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b7vxzxxdkxqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1bpat0h</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Birthday nails 🎂</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nv41lq22jxqc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1bpajmq</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Cut my nails short and did an eastern themed set. Should I add patterns?</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpajmq</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1bp9pj5</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Polygel nail techs in Vancouver, BC?</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bp9pj5/polygel_nail_techs_in_vancouver_bc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1bp82ta</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Chrome powder with Light Elegance gel?</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bp82ta/chrome_powder_with_light_elegance_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1bp797k</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Tried press on nails, liked them but……</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bp797k/tried_press_on_nails_liked_them_but/</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1bp6f8o</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Can you tell that these are store bought? I’m trying to justify if I should get my nails professionally done if these look tacky.</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bp6f8o</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1bp9j3j</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>2nd set of gel nails i’ve done on myself! Let me know what you think!</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bp9j3j</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1bp91ds</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Spring nails</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bp91ds</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1bp8szj</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>My client wanted something galactic. Do you like how it turned out?</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7chmti9r4xqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1bp8qzt</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>I've been trying to grow my nails out :/</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/95s2o8ad4xqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1bp7hid</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Non-greasy cuticle oils?</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bp7hid/nongreasy_cuticle_oils/</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1bp7dhb</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>advice needed for using magnetic polish..</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bp7dhb/advice_needed_for_using_magnetic_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1bp6j4q</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Short &amp; simple 🤎</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bp6j4q</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1bp6e3d</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>I’m dying ova here!</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vjb46gjenwqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1bp5hje</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Why are my nails chipping/peeling? I always have them painted.</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vomltb6tgwqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1bp5go5</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t xml:space="preserve">how do I paint my left hand </t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bp5go5/how_do_i_paint_my_left_hand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1bp5ylv</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>I feel strange wearing square nails again. How do they look?</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k6f934r9kwqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1bp0k40</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Polygel nails advice?</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bp0k40</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1bosm83</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Whitening Pencils</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bosm83/whitening_pencils/</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1bp59zg</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Had to do a sunshinepicture Hearts and Promises experiment polish she did hatchling #18</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/swxrgmibfwqc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1bp4dsn</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Is the tips too Big for my nails?</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bp4dsn</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1bp4auv</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Need advice</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bp4auv/need_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1bp3s1t</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>What are the different options to lengthen nails?</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bp3s1t/what_are_the_different_options_to_lengthen_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1bp3lq6</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Can I put my own nail decor at home after salon nails?</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bp3lq6/can_i_put_my_own_nail_decor_at_home_after_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1bp335k</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Builder </t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bp335k/builder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1bp30uv</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Resistance</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bp30uv/resistance/</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1bp2nqe</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Are these cute for easter or should I do something simpler?</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bp2nqe</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1bp2jr1</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Easter egg manicure done by myself *not a professional </t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oekdgguruvqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1bp25xz</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>What do we think? First try at 3D nails</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0nayix3prvqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1bp1mgz</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Forgot to post my christmas nails 💅</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bp1mgz</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1bp1ijl</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>How to remove lifted builder gel without starting completely over?</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bp1ijl/how_to_remove_lifted_builder_gel_without_starting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1bp0y6o</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>I am a Nail Artist👩‍🎨</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bp0y6o</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1bozbsn</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>is 6w uv lamp safe?</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bozbsn/is_6w_uv_lamp_safe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1boyt7b</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Black Cherry Berry nails 🍒</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1boyt7b</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1boyah3</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What does nail glue smell like? </t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1boyah3/what_does_nail_glue_smell_like/</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1bpq169</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Fast and simple</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpq169</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1bppzi8</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Lumen- Snow Shadow</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/av16xn1k61rc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1bppwmo</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>So I realized I own a color that almost exactly matches one of my favourite shirts...</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9hoqxlej51rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1bppa48</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Can anyone find a nail polish this milky, raspberry color?? It's to die for</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cjfcp6fgx0rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1bpp5mr</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Question about a red/pink iridescent red/pink nail polish</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bpp5mr/question_about_a_redpink_iridescent_redpink_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1bpopwl</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>ILNP Bluebird (perano blue)</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpopwl</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1bpobad</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Gel allergy havers- do your allergies or eczema flare up with self-made press ons?</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bpobad/gel_allergy_havers_do_your_allergies_or_eczema/</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1bpn4fx</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What colors should I get? </t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/64gkj9h090rc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1bpl8ho</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Color was prettier than I expected</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p86um2rzqzqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1bpk39u</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Can I use a gel top coat on press ons that are come pre polished?</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bpk39u/can_i_use_a_gel_top_coat_on_press_ons_that_are/</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1bpjj0s</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>PPU - Slumber Party Shag</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpjj0s</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1bpj323</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Indecisive 💚🩷</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/99k4mnwm8zqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1bpik3k</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>I’ll never NOT love this combo</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ya4w6s84zqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1bpihiy</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Grandma going silly</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpihiy</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1bphp5d</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Peep peep 🐣</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3sjdi90bxyqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1bphp37</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Pale pink jelly/crelly with red or orange shimmer?</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bphp37/pale_pink_jellycrelly_with_red_or_orange_shimmer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1bph3bt</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Easter Nails 🐇</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bph3bt</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1bpgwlv</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail hardener or nail oils? </t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bpgwlv/nail_hardener_or_nail_oils/</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1bpgrlv</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Lumen Besties… I’ve got mixed feelings</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpgrlv</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1bpgns6</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>First LynB Designs purchase and I'm in love with this iridescent bug color! ❤️</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rialczvepyqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1bpga29</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Hail the Sun Nails!</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpga29</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1bpcvry</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Synthetic Symphony is the bright purple I’ve been searching for 💜</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0m6nucfxxxqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1bpcph6</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>I think I just might be obsessed with reflective glitter now ✨</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpcph6</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1bpcnou</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>ILNP - Hidden Treasure</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1t91fxvawxqc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1bpcjuk</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Could my new holy grail quick dry, *non-yellowing* top coat be among these?</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpcjuk</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1bpc71s</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Cat Eye or Velvet?</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/991ghycwsxqc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1bpbnqs</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Needed to treat myself today #selfcare</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/no2rmyjzoxqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1bpba0p</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Good base?</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bpba0p/good_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1bpaznj</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Crackle nail polish vs gel</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bpaznj/crackle_nail_polish_vs_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1bpao8e</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>As neutral as it gets for me</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpao8e</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1bp9yx5</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>I subconsciously matched my phone!</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/itjx8fwucxqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1bp9xhf</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>I need to stop</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bp9xhf</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1bp8pyk</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>ILNP Poppy, I love it!</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bp8pyk</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1bp8xt3</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Rainy Reflective Skittle</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bp8xt3</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1bp8lkg</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>In love with this polish 😍</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bp8lkg</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1bp8agl</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>First time attempting Korean aura jelly nails ft Cirque Lavender Sky</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bp8agl</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1bp86w1</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Arwen</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y4oaprpc0xqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1bp7vhe</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Glass Frog jelly sandwich 🐸</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bp7vhe</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1bp7drn</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Finally got my hands on Pigeon 😍</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bp7drn</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1bp75sg</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Polish similar to LynB Apricity?</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bp75sg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1bp73t5</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Vivacious Violet</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/GkhHqRV</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1bp6xou</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Help me - split nail advice needed!</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bp6xou/help_me_split_nail_advice_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1bp6svu</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Easter nails 🐣</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bp6svu</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1bp5sef</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Nail repeatedly peels in same place</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kgat4bl1jwqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1bp5acc</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Had to do a sunshinepicture Hearts and Promises experiment polish she did hatchling #18</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/szu9i7gefwqc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1bp54hu</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Cracked nail 😭</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bp54hu</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1bp4scm</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>red mani. 💋✨</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bp4scm</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1bp4rol</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>My son let me paint his nails.</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bp4rol</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1bp43ik</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>This won’t be popular and that’s OK: Vanilla Bean nails</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bp43ik</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1bp42r4</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Easter egg nails!</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0frsmqxa6wqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1bp3u8x</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Emily de Molly "Half Orange"</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3gj8niag4wqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1bp2t13</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Are these cute for easter or should I do something simpler?</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bp2t13</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1bp2prq</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Looking for a flakey holo topper like KBShimmer’s flakes</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tb7vkuazvvqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1bp2asv</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>A New Favorite</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bp2asv</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1bp1r9o</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Long time lurker, first time poster</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ihbwyibovqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1bp15yd</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>A really pretty subtle thermal</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tcp1jvkcjvqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1bp0520</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Pretty Fly for a Cacti</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/whvomuup9vqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1boyy2y</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>First time using normal polish for a while!</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1boyy2y</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1bpprfb</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Evil eye </t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0olgzyco31rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1bpp6gi</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>They were supposed to be smiley faces but couldn’t get the mouth right so here we are ¯\_(ツ)_/¯</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpp6gi</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1bpougz</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Tying to improve my nail game.</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5z863rdgs0rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1bpm09s</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Glass Roses Tutorial</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://youtu.be/buZYxouOvNo?si=WyWAGYWYtJq34a-a</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1bpixni</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>most recent set I’ve done 💅🐱</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9kom5n0c7zqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1bph7s3</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Help! What am I trying to do?</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5hvkn0lktyqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1bpg02g</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Press on nails by sevennails</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z3m885khkyqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1bpb1vv</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Something fun for these shorties ✨</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b0zw8rnwkxqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1bp9kxr</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>2nd gel nail set on myself! Let me know what you think!</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bp9kxr</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1bp73u0</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Pastel Easter Nails 2024 with Born Pretty</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://youtu.be/gQf1ZG4eXFc?si=9GddVkhGoNqnypvh</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1bp6wna</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Chefs kiss 💋</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bp6wna</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1bp5iuf</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Easter 🐣 Nails</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bp5iuf</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1bp37we</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>trypophobia warning!</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w2w2txuwzvqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1bp10vf</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Feeling like Pablo Picasso👩‍🎨</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bp10vf</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1bowxvt</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>It was my experiment with long nails 🥹</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bowxvt</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Mar 29 08:08:13 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_03_31.xlsx
+++ b/data/2024_03_31.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C742"/>
+  <dimension ref="A1:C912"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13047,6 +13047,2896 @@
         </is>
       </c>
     </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1bqj1fv</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>This is beautiful 😍 - Nails by Annabel</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/szy8923s38rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1bq8xsp</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Builder gel changed colour, reaction?</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x89ahs1fk5rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1bq741z</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>I'm going to be doing my own DIY acrylics.... Which decals should I get? 3D Jelly flowers? or the Butterflies</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bq741z</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1bq5wra</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Extra long deco nails? J fashion trend</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bq5wra</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1bqa38r</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help me pick a color </t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bqa38r/help_me_pick_a_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1bqa5q4</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Has anyone used this?</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2g087ekkt5rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1bqhiav</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>How to fix dark cuticles?</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqhiav</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1bqbbdg</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Tried to make nails inspired by the trans moon flag</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqbbdg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1bqc4rz</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can I use Gel Glue on natural nails for gems? </t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bqc4rz/can_i_use_gel_glue_on_natural_nails_for_gems/</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1bqf09u</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>How do I get my nails to grow thicker and stronger 😭</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ga0g4ejlx6rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1bqgtij</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing my own nails </t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r4078eije7rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1bqgn6c</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>can never go wrong with the basic 🍒💅🏼</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqgn6c</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1bqge81</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Spring Nails</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqge81</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1bqg4vo</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Removing gems/stickers</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ki2a4rau77rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1bqfbk7</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Something fun for Sunday 🐰</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c5ehc3gg07rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1bqeq6a</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nails recommendation </t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bqeq6a/nails_recommendation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1bqeoi9</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Going to beach soon and wanted a tropical feel</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o6qxleapu6rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1bqejnu</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>how to prolong mani?</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqejnu</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1bqe3ia</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Are these worth 65 dollars</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqe3ia</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1bqdiu0</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Butterfly set 🦋</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1w5qlevqk6rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1bqdcyz</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Fresh mani + fresh pj's= happy me! 😻</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k0sv3bccj6rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1bqcmuo</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Look what I did!</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqcmuo</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1bqcapz</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Obsessed! ✨</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/eirdsj1fa6rc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1bqbrl2</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Got hard gels for the first time and all but 2 of my fingers have popped/lifted off</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a84esjw366rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1bqb0lr</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Inlay + Painted some butterflies on myself</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqb0lr</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1bqaiqd</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>I proudly present to you all: the best manicure I have ever done!! 💜</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqaiqd</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1bqa3sr</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Cat eye frenchies (kinda) with indoor and outdoor lighting done by me!</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqa3sr</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1bq9c1a</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Leopard Print Pink Press-Ons</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bq9c1a</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1bq99i7</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Teal? I usually do pink and I can’t tell if this is cute or not</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ntisdgum5rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1bq90ne</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>My first practice wheel is finished! Let me know your thoughts and ideas for the next one!</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bq90ne</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1bq8xo5</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Question for woc what nail color would go best with brown skin? </t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bq8xo5/question_for_woc_what_nail_color_would_go_best/</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1bq8vy7</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Some Press-On Sets I've done 💕</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bq8vy7</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1bq8r5p</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Any tips ton growing out my nails?</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7kpblhj0j5rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1bq7yfi</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Spring Pastel 💛🌷</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rh76z1jyc5rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1bq7ntv</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Spring nails!</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bq7ntv</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1bq7gbu</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Classic red for my 6th wedding anniversary on Sunday❤️</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3d3h0y0895rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1bq77rz</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Home self manicure</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bq77rz</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1bq6rn1</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>the afternath of a healthy acrylic removal + lots of nail oil !</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5fvu8q6845rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1bq6r5g</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>🤍</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rrbhbet445rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1bq68lm</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Nail anniversary</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bq68lm</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1bq5mki</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Did my nails for my dissertation defense!</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7s103td3w4rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1bq59fs</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Finished painting Nifty from Hazbin Hotel ✨</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7x668ebit4rc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1bq555v</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Designed some funky spring nails 🪩🌸</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uw977bens4rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1bq53mp</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Any advice / feedback?</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bq53mp</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1bq4uvv</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>4th DIY gel</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bq4uvv</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1bq4pfp</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do y’all have any tips on doing  Acrylic toe nails on myself from home? </t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bq4pfp/do_yall_have_any_tips_on_doing_acrylic_toe_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1bq4oj0</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Local nail salon got a new owner and 😍</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bq4oj0</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1bq49e1</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>easter nails!</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uu857a56m4rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1bq47mt</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Easter egg theme nails 💅 🥰</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bq47mt</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1bq44uf</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Nails that match this prom dress?</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p663skp8l4rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1bq3zxj</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Trying stickers</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/923b3g48k4rc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1bq3vpe</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>All my blue/green gel polish shades with a green pearl powder</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bq3vpe</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1bq3u9v</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Black is beautiful: black shorties.</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/etqgr262j4rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1bq3pyy</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>a few of my recent set as a 19yo beginner nail tech 🫶</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bq3pyy</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1bq3o58</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>I love this new 3d trend 🥰❤️</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/upukuidth4rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1bq34ez</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Numbers</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bq34ez/numbers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1bq344q</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>How bad do these look?</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lsf29e6ud4rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1bq2q8l</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Oranges that I did last night 🍊</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bq2q8l</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1bq2cs2</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Happy birthday to me 🦋</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bq2cs2</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1bq29vr</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>I was always curious why they’re called French</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1p00tnkz74rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1bq1xu5</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Blue 🩵</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5f97f9to54rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1bpzn1y</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7wtt4gh5p3rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1bpzlz6</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Mermaid DIY</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpzlz6</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1bpz8cn</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Tried to sculpt a bunny , can you see it?? Easter set</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpz8cn</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1bpxfqi</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>What is this?</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hkaeuxuo83rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1bpul9g</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>How to not get so upset over a break</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bpul9g/how_to_not_get_so_upset_over_a_break/</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1bpyspb</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Teal Chrome Press on’s</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpyspb</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1bpys3u</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Did my nails! ~Easter Vibes~ 🐰💜</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1sye16vvi3rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1bpyrlj</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Birthday nails ✨🩷💎</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpyrlj</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1bpynrq</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Peeling nails from buffing</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bpynrq/peeling_nails_from_buffing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1bpyljo</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Spring nails ✅</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1x2o8eaih3rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1bpyl2z</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Too Fall for Sprimg?</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ol6jqmaeh3rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1bpmt4y</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Not really Eastery but this is what I wanted for Easter</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpmt4y</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1bpy0e5</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>My first diy nails 🌸</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5jcdbqj0d3rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1bpi9g1</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Does anyone know where I can find sheer/jelly sage green or light purple *gel* polish?</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpi9g1</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1bpi3yc</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Am I doing something wrong? Which nail shape looks right?</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpi3yc</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1bphmu7</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>How do I fix this crack?</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xcsh26vrwyqc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1bpf2mx</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>abstract poppies done by myself//inspo</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpf2mx</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1bpdzz2</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bpdzz2/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1bpxbqf</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Egg nails!</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpxbqf</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1bpx434</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>First time getting nail extensions</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5vgk4qi663rc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1bpx3om</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Is bio gel the same as builder gel?</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bpx3om/is_bio_gel_the_same_as_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1bpx0kg</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>This is what perfection look like! Do we have here slim architecture lovers? 🔥</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpx0kg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1bpwgak</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>This is my therapy</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bjq5i6px03rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1bpu7d8</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🥹 my birthday nails, im so happy with how it turned out. Did took me hours to do, my hands are very shaky </t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4l7um51yh2rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1bptirk</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Can i have some KIND constructive criticism?</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/35olsu9jb2rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1bpt9n6</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>What went wrong? Newly bought gel nail polish (new brand) started looking like this after a couple of days and I have never had this problem with my other nail polish before. Bad brand? Didn't shake the bottle enough? Any ideas?</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2aiyh02292rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1bpt8f3</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sadness </t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/82ku3nhp82rc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1bpr0ti</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Did my own gel nails again - todays colour is Let’s Be Friends</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lc8h9dvpj1rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1bpqxma</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>some of the japanese style nails that i've made♥</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpqxma</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1bpqtsm</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Tips on how to make press ons not look like press ons</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hlhsuncbh1rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1bpqsqp</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Pomegranate nails</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpqsqp</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1bpq6yp</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>my simply pretty nails🤍</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p5tvmvmy81rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1bqc3vd</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Does the Nail magnetic work withany metallic chrome style t polish or chrome powder?</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bqc3vd/does_the_nail_magnetic_work_withany_metallic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1bqfvfq</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer - Amid the insects’ lulling serenade</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/s08xr3ti57rc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1bqfunz</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Looking for similar</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqfunz</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1bqfkh5</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Working on growing out my natural nails after 20+ years of biting and 8 years of abuse from getting acrylics / gel</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqfkh5</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1bqen14</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Is it ok if my cap doesn't cover the bottle's bottom ring?</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqen14</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1bqea8t</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rogue Lacquer Turquoise Mountain </t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/31xujm79r6rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1bqcedt</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Finally accepting lumen as a topper</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqcedt</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1bqcb3w</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>DVN Witches Slate</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqcb3w</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1bqbok9</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Dupe for Girl from Ipanema from Lights Lacquer?</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cchqbu8e56rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1bqbmza</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Easy sea glass nails</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a9qt3ab056rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1bq9q6h</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>A classic red mani</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oir7pjfaq5rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1bq9j41</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Mobius in velvet</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bq9j41</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1bq404d</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>What color would look good on my skin tone?</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bq404d/what_color_would_look_good_on_my_skin_tone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1bq8zpa</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>More PPU- Like Magical Gumdrops!</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d74w75trk5rc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1bq82y1</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Opi: Mexico city move-mint</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6kyp70gwd5rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1bq82f4</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Question about Ella + Mila First Aid Kiss</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bq82f4/question_about_ella_mila_first_aid_kiss/</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1bq7ub1</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>OPI "this color's making waves"</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bq7ub1</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1bq7cx8</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Sometimes color inspo comes from the craziest places</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/2nCuHLG.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1bq72eh</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>DVN Limerence is the color of spring</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bq72eh</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1bq6yxy</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>What Addiction? - Nocturnal Deathstalker PPU February 2024</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bq6yxy</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1bq6gtl</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>New set since yesterday</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bq6gtl</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1bq67xl</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Easter Extravaganza</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bq67xl</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1bq5q41</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Organizing polish without #'s or cap stickers</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bq5q41</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1bq4kc2</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Lava Lamp x Mermaid Grotto</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bq4kc2</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1bq4i70</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Three Months of Garden Path Lacquers PPU</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/10u4hd10o4rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1bq4i4b</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>nail drying help</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dhn0kxoyn4rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1bq4av7</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>NeVerMind Holo Mani</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bq4av7/nevermind_holo_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1bq3nmo</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Not sure about this one</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bq3nmo</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1bq3k9l</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Yellow, my friend⭐️</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7bbiz282h4rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1bq3ifk</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>ILNP Pink Suede 😍</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bq3ifk</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1bq3g8n</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Morpho glow + moon ripple</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bq3g8n</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1bq2bri</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>The difference light makes. 🤯</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bq2bri</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1bq25jh</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>The stray cat hair adds that perfect touch</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oj6n0qa674rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1bq20qr</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>This one blew me away 💜💜💜</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bq20qr</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1bq1ir5</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>What to do with peel my base when it gets low?</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bq1ir5/what_to_do_with_peel_my_base_when_it_gets_low/</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1bq17ug</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>10mg of adderall</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ohfy94nk04rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1bq163y</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Blush nails and an attempt at stamping</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wtpgqy7804rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1bq11rf</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>5 day old first attempt at nail art 🍬 any easy beginner looks to try next?</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bq11rf</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1bq08q6</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>🔹One Coat Wonder🔹 Blue</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/CaBhWqH</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1bpzuez</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>the sky above</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qr30ybjmq3rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1bpztjs</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>What are the differences between all those store polishes like OPI, Essie, Orly, etc vs brands like Mooncat, Holo, Cirque, etc?</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bpztjs/what_are_the_differences_between_all_those_store/</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1bpz2hy</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Coffee themed nails</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpz2hy</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1bpoz56</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>OPI Yogata Get This Blue Vs. Chopstix and Stones</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bpoz56/opi_yogata_get_this_blue_vs_chopstix_and_stones/</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1bpxksq</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Self tanner stained manicure - any solutions?</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bpxksq/self_tanner_stained_manicure_any_solutions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1bpx7ua</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Beginner nail art (subtle pastel tips)</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/myhjixiy63rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1bpvqom</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>So excited!</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpvqom</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1bpv8ei</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>I bought the nail rings</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpv8ei</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1bpul08</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do you have a color don't like but you still try it every so often? </t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eggnhwdal2rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1bpukkl</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Shooting Star so pretty!</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpukkl</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1bpuc7r</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>LynB Slumber party shag (ppu)</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpuc7r</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1bprqb7</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Bluesky - Quiet Grey</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x58v84ges1rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1bpqone</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Gel manicure for my holiday!</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpqone</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1bpqhjz</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Please, help me find this colour!</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jdqxi5zvc1rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1bqj04k</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Nails to go with henna</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aejy9jch38rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1bqgqq8</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>peachy sultry nails</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqgqq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1bqfkel</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>I feel like a kid, these are awesome! 🤣</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqfkel</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1bqebku</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>100% neon design</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqebku</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1bqe09c</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Pokémon nails</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/74nett1vo6rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1bqbrck</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Cloud and Pearls</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqbrck</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1bqatxe</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Two more of my designs :)</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4wzdi14oy5rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1bqascd</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>First practice nail art wheel done! Send suggestions for the next one!</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqascd</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1bq9gce</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Shinobu Butterfly - DemonSlayer 🦋</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kp1f6p1ao5rc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1bq8ho2</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>First attempt at drawing stars!</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bq8ho2</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1bq869d</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Easter Nails 🐰🐣</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ncd8nhke5rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1bq7x37</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Spring nails🌸🦋</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bq7x37</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1bq7wzj</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Easter set by @NailzXshanti</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bq7wzj</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1bq5abq</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Finished painting Nifty from Hazbin Hotel ✨</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rpet6bzot4rc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1bq45jg</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Spring polka dots</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cjqnjnfal4rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1bq3j4s</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Mini eggs 😋</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ipyjmgbug4rc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1bq102g</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Practicing on my best fran</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2n6w4gszy3rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1bpzfb7</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>I attempted to sculpt a bunny</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpzfb7</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1bpypfo</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Spring Butterfies</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/59rdg1ubi3rc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1bpyl66</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Set for my little bestie </t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pk7nuh4fh3rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1bpwwef</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sanrio Inspired </t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ydwn3e2j43rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1bpwto7</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AOT inspired </t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7op38nkx33rc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1bpu5gv</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Easter nail art</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpu5gv</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1bpr77i</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>It’s like liquid steel 🥹 what do you think about my work?</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bpr77i</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Mar 30 08:07:43 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_03_31.xlsx
+++ b/data/2024_03_31.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C912"/>
+  <dimension ref="A1:C1072"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15937,6 +15937,2726 @@
         </is>
       </c>
     </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1brcii1</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>New Set</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o7qt7auygfrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1brchqh</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>First time using biab</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brchqh</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1brc9il</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Easter manicure 🐣</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qxktzhlxdfrc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1brbpmc</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>pink floral nails - self done 💕</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brbpmc</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1brbz24</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Love it, wish I went longer💟💟</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yp4mhd8hafrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1brbszx</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Nails I Did for my Aunt!</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kqy3s1ak8frc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1brb8uf</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Easter nails</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brb8uf</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1bralze</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>only starting ti get into simple nail art for fun, really starting to like it!! ⭐️ 💅</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r7nprjs8verc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1bra69h</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>My first time ever working fake nails and charms</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bra69h</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1br9x33</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Does anyone else have a single nail that grows in weird?</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1br9x33</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1br56we</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>How to change nail bed shape?</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1br56we/how_to_change_nail_bed_shape/</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1br403r</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Some nail art I did when I was ~16 vs. how I wear nails nowadays</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1br403r</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1br3r12</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Help! Gel caps vs gel nails</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1br3r12/help_gel_caps_vs_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1br36q5</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Gelish Nails Gel Polish Lifting</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v7q0hnwh0drc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1br8tp2</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Ready for spring 💅🏼</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j2h7a2l3derc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1bqxkzh</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Mini Egg Inspired Mani for Easter!</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kwbn4xeurbrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1br8s43</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>First time having my nails done since the divorce</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sdxniyfocerc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1bquzca</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Is it obvious I’m inspired by Korean nails? 🌸</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bquzca</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1bqtfwa</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Where should I get my nails done in LA?</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bqtfwa/where_should_i_get_my_nails_done_in_la/</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1bqsnbx</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Nails after acrylic</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqsnbx</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1bqrsue</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Spring nails🌸💙🤍</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u2s9kklmiarc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1bqrpos</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>How to apply nail polish smoothly???</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bqrpos/how_to_apply_nail_polish_smoothly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1br8g6l</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Fresh set 😍🥰 Done by @nails.by.carla_ on IG!</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iv5pfmvi9erc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1br88ne</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>cutest set</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/exvu1k9i7erc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1br8155</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>My first gel ex nails that i did myself!</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oy6jyrdk5erc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1br80vw</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Easter nails🐇</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1uy14xdg5erc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1br7vcp</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Classic</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yl2hwo704erc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1br7k3i</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Recent structured gel manicures I’ve done 💫 (all their natural lengths)</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1br7k3i</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1br7c19</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Does anyone actually take a break from acrylics?</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1br7c19/does_anyone_actually_take_a_break_from_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1br6y49</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Wanted to share my previous set 🖤💛</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/llm09wxlvdrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1br6r0e</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Is this normal?</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ribygdystdrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1br6oqg</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Melty Frenchies 😍</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5jw252j8tdrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1br6jgh</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>I think these are my favorites ever</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1br6jgh</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1br6i9t</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>I'm in love!</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1br6i9t</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1br67ki</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>How to fix my nail beds</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1br67ki</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1br5qij</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set. I was feeling springtime </t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uxyj4i93ldrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1br5exe</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vxacvzedidrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1br5bn1</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>literally so pretty 😻</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1br5bn1</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1br4cmx</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Pixie Party</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1br4cmx</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1br49lw</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Blueberry Nails 🫐</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/guugz13x8drc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1br3w1d</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Finally getting a little bit of length back.</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1br3w1d</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1br3np6</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Did I just get a bad French manicure?</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1br3np6</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1br3jnk</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>we like?</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1br3jnk</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1br3b5u</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Slowly making its way into my heart at my fav spring set ever (had to delete other post to remove nail salon number)</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/41nnzefg1drc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1br2npz</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Milky natural 🥛❄️</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1br2npz</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1br2g4b</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>I’m so in love with the plain Jane ✨</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9fn0rac0vcrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1br2762</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Regular clear polish over gel</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1br2762/regular_clear_polish_over_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1br21op</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Tried a plastic wrap inlay on my guy friend. Turned out alright!</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1br21op</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1br1tsl</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Purple and Pink Nails</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aatlq80hqcrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1br1dwc</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>🌸🎀💐pink !</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1br1dwc</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1br1a0s</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Rainbow smoke</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1br1a0s</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1br0xyu</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>I will always choose milky white over white🥛🤍 self done</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1br0xyu</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1br0rsr</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Any other guitar long nail girlies?</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1br0rsr</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1br0nwh</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I loved this cute design and color combination </t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1pu7znv3icrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1br0g1s</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Cat eye</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8n1738kjgcrc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1bqzrti</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Cowboy Carter Beyonce themed nails by me 🤠</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqzrti</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1bqzqqa</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>BCB Lacquers - I'll Never Go Back on My Word 💛❤️‍🔥🧡</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqzqqa</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1bqzpgb</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Officially spring ready. </t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u1snm9qebcrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1bqz47b</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>This pink shimmers in any lighting 💅 [F] [Pink]</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jdw21yxs6crc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1bqypsz</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Easter nails</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqypsz</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1bqyadm</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Do you think this nudie pink matches my skin tone? I think I might’ve found the one!</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqyadm</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1bqy7lm</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Steampunk &amp; Bumble Bee Gel Stamping over CatEye Gel</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqy7lm</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1bqy4mc</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Help finding good products for dip nails</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bqy4mc/help_finding_good_products_for_dip_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1bqx4ur</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone else end up destroying their nails when they try to do an at home manicure? </t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bqx4ur/does_anyone_else_end_up_destroying_their_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1bqx4t0</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone else end up destroying their nails when they try to do an at home manicure? </t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bqx4t0/does_anyone_else_end_up_destroying_their_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1bqx4ej</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>First go at long squares</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqx4ej</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1bqwnlk</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>green 💚 done by me</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fyc7h5g8ibrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1bqw8cr</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Natural Nails w/ Gel Art🌟</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ntkpbl16fbrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1bqvuwj</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>I can't stop looking at this mani</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n0wwnivhcbrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1bqvjfe</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>New Nails💅</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tos8co17abrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1bqv882</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>I feel the color doesn’t match my skin, what do they say?</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aty2ut4v7brc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1bqtt3c</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Always wanted to try these 🥰🐍</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqtt3c</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1bqtjtp</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Hoping these spring nails will bring better weather on the East Coast!</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dksxci5lvarc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1bqtiap</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>One short nail.</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mmvrzql9varc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1bqt27n</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Loving my new set!! 🤘🏻</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqt27n</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1bqsvva</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>I've been loving this manicure I did on my natural long nails</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqsvva</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1bqs7mf</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>New nails! I love them 🩷</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tbwesl0olarc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1bqrr1n</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Robin’s Egg nails!</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vv3b07u8iarc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1bqrhwi</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>needing advice / tips</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqrhwi</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1bqr3uf</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Heart broken</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vsvtmapfdarc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1bqqv5k</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Should I try other color?</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p0fvrubmbarc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1bqqgl9</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Application Timing</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bqqgl9/application_timing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1bqqfb5</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>tried to remove my rubber base gel overlay and this happened :(</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zu02xio68arc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1bqq34c</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Bright &amp; florals for Spring ❤️ love them</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s4yrnfuh5arc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1bqppvb</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>How often can I do builder gel?</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bqppvb/how_often_can_i_do_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1bqpn6o</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>This has to be my favorite set!</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqpn6o</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1bqoghb</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>can I fix these bubbles or should I just start over?</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqoghb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1bqnkbm</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My friend said it’s giving “excited for the eclipse” lol I’m obsessed with them regardless </t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pzjog9itj9rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1bqmcu5</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Bee's Knees Lacquer - Wyrd</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqmcu5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1bqmbzh</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Modified French nails done by me 🩷</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ka1681jg79rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1bql584</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>I finally got the nails I've wanted</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uu6xz9bvt8rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1bql501</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Color changing nail polish 🙏</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/eg0y2zist8rc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1bql3qi</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Really proud of this as a beginner nail tech :)</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6pz569gct8rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1bqkpdr</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spring nails </t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/58wc63mmo8rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1bqkgk3</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>My first poly gel set</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqkgk3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1bqkdx4</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Spring Vibes💚</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ltr0oi1sk8rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1brb46k</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Easter nails</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brb46k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1brauy0</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Attempting opal nails</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brauy0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1br7rqs</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>BKL Through love, all is possible</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dp4o9ev23erc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1br7m3w</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finally getting the hang of the filing them </t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/unc9b4cl1erc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1br6oji</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Spring nails with water decals</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/95si00w6tdrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1br6fpb</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>It's giving Slytherin 🐍</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1br6fpb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1br2iyc</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>What a great neutral pink ☺️ Polishes Used: ILNP (Shade: Sweet Pea) | Essie (Shade: Gel Couture Top Coat)</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1br2iyc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1br2f0t</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>You can never have too many shimmery pinks 💖🧚🏼‍♀️ Polishes Used: ILNP (Shade: Pixie Party) | Essie (Shade: Gel Couture Top Coat)</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1br2f0t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1br5ybq</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Toe Beans with Toe Beans</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/afwg5ulxmdrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1br5y91</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Before &amp; after polish 💖</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1br5y91</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1br5j5a</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>LynBDesigns!</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1br5j5a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1br4wen</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Time for some spring nails </t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8xo1k6b7edrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1br4i2m</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Easter nails</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b78s0l1uadrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1br4c7f</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>A fleeting shower thought</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1br4c7f/a_fleeting_shower_thought/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1br46s5</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Was trying to find the right lilac color for Easter…</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ndezgr98drc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1br41uf</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>✨️✨️Pixie Party✨️✨️</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1br41uf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1br3bdu</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Marbled nail skittle (a first attempt)</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1br3bdu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1br2r64</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Witchcult mystery Janette charity polish</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ivdn9kqaxcrc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1br2iqj</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Ethereal- Calcifier</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p8o22c7jvcrc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1br1sag</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving the copper flakies </t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p6uxdwi6qcrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1br1qd9</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>My attempt at Easter nails!</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1br1qd9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1br1lw8</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>A kitchen mishap only TWO days after a big chop :(</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1br1lw8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1bqz9iz</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Doing nail art while sick hits different 🤧</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ru1d7pk88crc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1bqywd9</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Well, A for Effort at Least </t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ycc1k6kk4crc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1bqytzp</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Matches my dress perfectly </t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8qyn6w3w3crc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1bqytly</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>More sagey gray in direct sunlight, Birds Fly by Phoenix</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqytly</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1bqyquc</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Girl Talk ✨</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqyquc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1bqyia3</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>BCB Lacquers - I'll Never Go Back on My Word ❤️‍🔥🧡💛</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqyia3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1bqy800</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Fingers crossed for me!</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/myl20f9oxbrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1bqxmzd</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>2nd edition of “You already know what this polish is, don’t you?”</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqxmzd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1bqxc60</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Oreo nail art with the new Holo Taco polishes!</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lnpaeatcpbrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1bqvz8x</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Old manicure (before breaking my nails 😭)</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqvz8x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1bqrukj</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Easter nails 🐥🐥</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqrukj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1bqvmmy</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>BKL Choose Life makes a perfect velvet</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqvmmy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1bqvfkv</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Trying my best to summon the Easter Bunny with my nails 🐰</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yop3jxre9brc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1bqvalu</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Mooncat Blame My Star Sign (and a Pretty Grunge cameo)</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqvalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1bqv4xv</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Let's go Sabres 🦬</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vjk6kbyt6brc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1bquzjk</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>First time painting nails in a few years</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bquzjk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1bqux80</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>One week of Lucky 13 - The Secret of NIMH</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/37mxf75q5brc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1bquca2</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>All I wanted to do was scratch my back 😭💔</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/302ax00f1brc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1bqtfqx</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>colorful tie dye french for easter 🎨🐣</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p87s5mmquarc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1bqt3m7</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>💫🌟✨</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqt3m7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1bqt2u9</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>My take on Easter Nails</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5uqjqhj3sarc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1bqsvkh</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Going speckled for Easter 🐣</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqsvkh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1bqssiv</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Color Club - Blue Heaven</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqssiv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1bqsek1</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Keeping my nails protected (and pretty) while painting and moving</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqsek1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1bqs0dp</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>LL La Luna</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bqs0dp/ll_la_luna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1bqrvui</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Easter Mani ft Cirque Stoneware matte</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqrvui</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1bqrk15</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Playing with Purple 💜</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/udp6obkrgarc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1bqr50x</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>tried to soak off my rubber base gel but it still peeled like this 😭 what can i do while it grows out?</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yxydzgyodarc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1bqqzui</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>BKL - She Was Enough</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqqzui</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1bqq4uu</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Spring pastel jellies 🌸🌱</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xj8s3du65arc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1bqkbo8</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>First freehand art!</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/er4se682k8rc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1bqpr5u</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Found a relic at the thrift store today!</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tovagkcx2arc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1bqo7rc</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Maybe I went overboard</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqo7rc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1bqmmvf</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Baby Pink</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqmmvf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1bqmbzu</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Bee's Knees Lacquer - Wyrd</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqmbzu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1bqkdd5</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Spring vibes💚</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lqhdu11mk8rc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1br5cw8</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press on set </t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bxkio7exhdrc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1br1bvy</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Jelly and chrome pastels</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e6qqns2wmcrc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1bqzsq0</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Cowboy Carter Beyonce nails by me 🤠</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqzsq0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1bqwjdo</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Nails (loosely) inspired by Julio Torres’ Problemista 💅 ✨</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqwjdo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1bqv1a8</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Korean nails inspired me 💅🏼</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqv1a8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1bqrcjc</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Remember when you were a kid and you’d squish all your Playdoh together?</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bqrcjc</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Mar 31 08:07:46 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_03_31.xlsx
+++ b/data/2024_03_31.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1072"/>
+  <dimension ref="A1:C1253"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18657,6 +18657,3083 @@
         </is>
       </c>
     </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1bs57wi</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Disco nails 2.0!!</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bs57wi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1bs57nr</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My fist ever set as a nurse, I love it </t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fq3v7ua7nmrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1bs53c9</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>BIAB progress continued including accidental 5+ weeks growth</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bs53c9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1bs4uio</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Budget nails: Cheap plastic press ons (with gel)</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bs4uio</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1bs28lg</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Do these look chunky??</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6zg207q8plrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1bs1onu</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>first set of press-ons</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bs1onu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1bs1eqi</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Cheetah Print Nails!</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/20ct742vglrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1bs0sr7</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Sculpted Polygel 🌸🐰🌻</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bs0sr7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1bs0fqd</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>What colors do you guys think I’d need to recreate this sky on a nail?</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/23ivxdgs7lrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1bs0bkl</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What would y’all do for an eclipse theme? </t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bs0bkl/what_would_yall_do_for_an_eclipse_theme/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1bs05su</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>My latest custom press ons</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bs05su</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1brzpr5</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Coming out of retirement to work at home.</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1brzpr5/coming_out_of_retirement_to_work_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1brzpqd</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>New Nails</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/79l16rq51lrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1brzl07</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>best affordable nail builder gel</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1brzl07/best_affordable_nail_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1brzjgi</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Glittery white nails for Easter/Spring 🤍✨</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xu0i7vslzkrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1brzgwg</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Baroque</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ewzidvkzykrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1brzfay</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Clear/Natural polish recommendations?</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brzfay</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1bryoae</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>New chrome set today!</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/si7qkyourkrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1brxrzb</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Spring 🩵🩷💛💚🤍</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brxrzb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1brximu</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>cute minimal claws</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brximu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1brwz0o</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>First time doing gel nails on someone else!</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brwz0o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1brwe2p</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My boyfriend wanted to match me so I did our nails &lt;3 </t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t8uog8ft8krc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1brw0jc</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>My new cat's eye mani with cool flowers made from a magnet. I'm so obsessed with this type of polish!</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brw0jc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1brvebc</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Hand-Painted Art 🎀</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brvebc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1brvbll</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>evil eye nails 🧿</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brvbll</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1brv8gh</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Builder gel lifting. </t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fmvng9ppzjrc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1brut7k</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Spring frenchie</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ituvow4fwjrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1brur2w</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>How often to replace?</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brur2w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1brung4</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Surrealist nail art today</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brung4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1brumdd</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Fave at-home nail color routine?</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1brumdd/fave_athome_nail_color_routine/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1brulno</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>First set in years!</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brulno</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1bru5b3</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Are my nail beds too wide?</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gj6s0f6drjrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1brtvhx</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Butterfly nails</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/qxOgGD7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1brtskt</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>First chrome set ever! 😍</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nczrehgmojrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1brtlbn</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Weekend Nails</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3g2e1y44njrc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1brtfof</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Red ❤️❤️❤️❤️</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xdha222wljrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1brt7zr</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>So happy with how these came out!</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xlbjn725kjrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1brsw0q</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Birthday nails to match my birthday outfit</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h3wec1zqhjrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1brs90p</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>I love this dark vibes</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iu6hud9xcjrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1brrtww</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Sailor Moon inspired nails for my bday! By okenails in Brooklyn</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brrtww</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1brrf8c</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>how do we feel about these nails?</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9c58qhkm6jrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1brs3t8</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>I’m so sad but</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1brs3t8/im_so_sad_but/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1brrzij</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>I give up</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1brrzij/i_give_up/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1brrvlj</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Bright tips for spring!</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brrvlj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1brrt8l</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Dip Powder</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1brrt8l/dip_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1brr6am</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>✨Etsy pressies✨</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p9e62glr4jrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1brr3cn</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Red and black punk nails</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0r35exk34jrc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1brr20x</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>💚🩷</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brr20x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1brr01u</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Prom nails?</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1brr01u/prom_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1brqsvg</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>easter nails 💜🦋</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/19hhw4lw1jrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1brqct7</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>How does this look? Just got this manicure for $28 at a local salon. Opi base and top coats, Essie Gel Couture in Sheer Silhouette for color.</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brqct7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1brq4pu</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>🩵 Painted Polish Once &amp; Flor-al💜</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brq4pu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1brpzfh</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>can you apply soft gel nail tips with regular nail glue?</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1brpzfh/can_you_apply_soft_gel_nail_tips_with_regular/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1brpsr3</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>💗💗💗 I love this my work</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brpsr3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1brphwi</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>how much would acrylics like these cost??</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/frh4wgfurirc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1brp8co</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cute spring toes! </t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e2t6yl4rpirc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1brp2x7</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>How to remove shine from acrylic on nails.</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cdd8o3fmoirc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1brp2gx</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kiss Impress nails </t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1m249vgjoirc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1brp154</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Nail Biting Q&amp;A</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1brp154/nail_biting_qa/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1brow8q</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>I’m so in love with the nude look 💖🥰</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bxjb8o08nirc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1bror2o</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Classic 💅</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hauckef3mirc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1brombd</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Why do they look off?</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brombd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1broliq</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Presson set by me 💟</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1broliq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1brofze</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>New nails!</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/arw8aa3tjirc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1broemn</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Monochrome set I did on my client!</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ibes7zjjirc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1brngpt</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Olive my new manicure</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brngpt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1brnbfw</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Best Nail Salon for damaged brittle nails ?!</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1brnbfw/best_nail_salon_for_damaged_brittle_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1brn95u</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>I love having many colors</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nths0ndsairc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1brmxuc</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>I mixed these two together and I'm obsessed with the result</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zemrq5me8irc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1brlzyg</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>french mani done by me ON me :) (no im not ambidextrous, yes this took hours)</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brlzyg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1brluua</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>💙</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brluua</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1brlrll</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>best biab nails in birmingham uk??</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1brlrll/best_biab_nails_in_birmingham_uk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1brl7y2</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>I hate them lol 😆</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eg9t2z81vhrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1brl7eg</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>My kind of spring shade 💜🔮</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lye1vtexuhrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1bre0s6</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>how to fix years of nail biting</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bre0s6/how_to_fix_years_of_nail_biting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1brj6ha</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>why is my rubber base gel turning white after curing? is it normal?</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sv40if4xehrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1brhjmu</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Spring nails🌼</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ckjlyt1y0hrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1brkrcd</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spring nails! </t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aq9gdx8irhrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1brkhkh</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Easter nails I just did! Bit shaky, but considering that I don't do much nail art and you need to work quick with normal polish, I'd say I'm pretty proud :)</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brkhkh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1brk4eb</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>First XS Coffin Set for Easter</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brk4eb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1brjxft</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>I call this little number “to swim in the sea, like I walk on the shore”</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brjxft</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1brjp5v</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Back to shorties for the landscaping season</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brjp5v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1brjhah</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>So happy with how these turned out!</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brjhah</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1brjgao</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Manicure nail growth progress 🍫🌰🌺🩷</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hm3rjk84hhrc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1brjfny</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>First time ombré acrylics</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3o5bgaizghrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1brjc0i</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Last months mani</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f20mp0n5ghrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1brip48</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Second Gel Mani after all of your tips!</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wss5gf2wahrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1brifgd</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Second time using biab</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cd1e5qlo8hrc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1brhr21</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Unicorn Cat Eye</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/a0zf1o0t2hrc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1brgqg1</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Red nails this time</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lky68mkftgrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1brgnim</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Late valentines set</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eu884n1osgrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1brfr6e</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Hard Gel nails for soft natural nails…..</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1brfr6e/hard_gel_nails_for_soft_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1brffep</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>New nails for spring! 🥰</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zlzp2hq8ggrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1breq47</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Did myself french. I can do french))</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zn47f4c68grc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1bre86j</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>I love butterflies 🩵🦋</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bre86j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1brd190</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>new nailsss!!!🌸</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4z2zc0venfrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1brcq1c</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Happy Easter 🐰</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u9nz9o5ijfrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1brcnzs</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Started to do my own nails.</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brcnzs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1bs41xg</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>🌈🐘🌈🦏🌈🦛🌈🦍🌈</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bs41xg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1bs37v9</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Quick swatch of the Ethereal Calcifer mystery, She Likes My Spark</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nk8y2ktxzlrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1bs34on</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Molten Lava from Mooncat</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bs34on</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1bs31yh</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Maybe there is something to this car lighting thing!</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bs31yh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1bs23g1</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Fell in love with these too late- what are dupes that are available?</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bs23g1/fell_in_love_with_these_too_late_what_are_dupes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1bs1u4i</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to get color accurate photos/video? </t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/17nlhp1zklrc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1bs0h4n</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Phoenix polish chibi chibi glows💖</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bs0h4n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1bs041o</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Is this velvet? I'm not sure I get it</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qtx5el2t4lrc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1brzy0u</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Blue and rainbows, two of my favorite things!</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brzy0u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1brz1kg</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>How to regrow?</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wzz9n8u1vkrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1brybsm</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>I don’t usually love reds on me, but I make an exception for this one</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brybsm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1brxgb0</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Poparazzi Noble Quartz is amazing!</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/as0ee65ghkrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1brx514</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>I tried nail art for the first time. 🐣</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brx514</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1brx0lk</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Was about to destash this lacquer, but now obsessed with it as a topper</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brx0lk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1brwla0</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Polished for Days - Blossom 🌸</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brwla0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1bruw4j</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Dupe for Cirque Introverde?</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bruw4j/dupe_for_cirque_introverde/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1bruod0</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Spring in a bottle (and now on my nails)</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/grm35ooevjrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1brue98</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Trouble with cirque peel off base?</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1brue98/trouble_with_cirque_peel_off_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1brubio</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>His Monstrous Queen 👑</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brubio</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1bru52m</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>OPI Summer 2024?</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/76xc4r9brjrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1brteyc</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Can someone invent a ring that holds cuticle cream please</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1brteyc/can_someone_invent_a_ring_that_holds_cuticle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1brsxu3</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>What I wore in March</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brsxu3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1brsxe8</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cut protection? </t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1brsxe8/cut_protection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1brsovf</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is this salvageble? </t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6lj9j3b9gjrc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1brsocr</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Searching for more lighter olives to add to my polish collection, does anyone have any recommendations? They can be of any finish.</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0mdv9f0yfjrc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1brsl7u</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best way/direction to file free edge </t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1brsl7u/best_waydirection_to_file_free_edge/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1brrwok</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Spring nails! 🌸🌸</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brrwok</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1brrke3</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>this month’s nails: march 🌱</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brrke3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1brr67u</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>This is only my 3rd time using gel polish. I've been using some cheap set I got off Amazon "gelen" and it tasted for about 2 weeks. I then got some beetles matte,top,base, and black for this. Not even 24hrs later and it's chipped and I could just peel off the whole nail. Did I do something wrong?</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0bz72ico4jrc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1brnkea</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Weird Q re thermals</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1brnkea/weird_q_re_thermals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1brqn38</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>ILNP - Paisley/Fairy Dust</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i2k8nn9o0jrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1brq2e9</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>🩵Painted Polish Once &amp; Flor-al💜</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brq2e9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1brpu8w</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Sunny spring sky nails 🥹 (feat sleepy baby)</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qnmob5yfuirc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1brphr2</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🌼 periwinkle 🌼 </t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qdmf0y2trirc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1brnpeu</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Quail egg mani</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brnpeu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1bromh6</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Sparkles for Easter!</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6u5g9ka5lirc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1brok3d</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Easter Nails feat. Emily de Molly</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brok3d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1broe7r</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Nail help!!! :(</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1broe7r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1brnm1t</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Calcifer! 🔥</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brnm1t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1brnjbn</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Couldn’t decide, so I did … everything?!</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brnjbn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1brlxyb</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Has anyone tried water marble technique with Jelly polish (cirque colors)?</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1brlxyb/has_anyone_tried_water_marble_technique_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1brlwl2</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Chibi chibi needed something …so on went one coat of Ether Dragon! CUZ SCIENCE and i definitely like it better now 🤓</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2an7kkha0irc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1brlqcj</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>{PR} What a Pearl Wants by KB Shimmer</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y9lnsrhyyhrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1brlkdm</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Cirque Colors - Ghost Rose</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brlkdm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1brldhw</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>✨️🥣Cinnamon Toast Crunch🥣✨️</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brldhw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1brl56s</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>My kind of spring polish 💜🔮</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9vfic0aguhrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1brkubh</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>BKL Easter Skittle</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zlykhxv4shrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1brkmzp</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>I just can't stamp over this!</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/feenwz5mqhrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1brkhsy</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Learning to do the nails myself</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brkhsy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1brkbw6</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Not a good quality, but I love the color ^^</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brkbw6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1brk5ei</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Obsessed with thermal polish</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brk5ei</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1brk2fr</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Magic in a bottle🧚</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brk2fr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1brk0k0</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Stiletto</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1brk0k0/stiletto/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1brjtlk</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Lush by PFD</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brjtlk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1brjo8n</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>My mom got me some cute little nail stickers.</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brjo8n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1brjnr2</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Easter nails</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7zo5kb3tihrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1brjlmj</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>This one looks so good in any lighting, I'm obsessed</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brjlmj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1brivsr</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Mooncat newbie</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6gg1leffchrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1brii4x</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Across Time or Devils Ivy for Easter?</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lo0vpcrb9hrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1bri5bb</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Second attempt at polygel :(</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bri5bb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1bri064</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Couldn't wait to use my new stickers</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h588m1015hrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1brhyh3</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Daisy Nails</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brhyh3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1brgxou</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lurid Lacquer - Amid the insects’ lulling serenade (Daylight) </t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6mwskkoavgrc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1brfqi5</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Therapy</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1brfqi5/therapy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1brd7ri</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Tell me it’s ok if I never finish a bottle of polish.</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1brd7ri/tell_me_its_ok_if_i_never_finish_a_bottle_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1brd0zd</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Is there any benefit to adding squalane to my nail oil?</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1brd0zd/is_there_any_benefit_to_adding_squalane_to_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1bs3ohz</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Strawberry/Cherry Nails!</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rses0wm55mrc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1bs2j0p</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Nails done for my aunt!!</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yeg8yql8slrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1bs2ihj</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Any tips for a beginner</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bs2ihj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1bs1wvf</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Not my best work :/</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bs1wvf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1bs1op4</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>I did a different style of nail art for Easter and I don’t know how I feel, advice?</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nwwh8sxhjlrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1bs1cj8</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Can you guess the theme?</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bs1cj8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1brxyoz</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Here’s my attempt at cottage-core nails spring nails✨🍓🍄</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tzx422eolkrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1brwtl1</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Another pinterest-inspired set for me this week!</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brwtl1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1brt0vc</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails lila </t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/buTIlt0.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1brrehi</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Hand painted Easter nails 🐰🐣</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brrehi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1brpl7v</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>It’s so cute 🥹</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m9d9scdksirc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1brpkdc</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>First attempt at nail art following a tutorial. I was unsure at first but they aren't too shabby! Tips for next time?</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brpkdc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1brpfnz</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Chunky Funky Spring Butterfly Nails</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://youtu.be/eEIZbqjsd8g?si=XOauvp1Ftvqv-3PA</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1brm0hn</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Officially strawberry season🍓(credit:Myself)</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g7g0xxk51irc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1brla8x</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>I'm Mr. Meeseeks look at me!!</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aactpiehvhrc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1brko4g</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Easter nails! I don't typically do nail art so these are a bit shaky but I'm still pretty proud :)</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brko4g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1brjwku</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>I'm super proud of these adorable Easter nails. What are you all doing for Easter/spring?</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1brjwku</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>